<commit_message>
Testcases file (rev02_testcases_20200729.xlsx) update
</commit_message>
<xml_diff>
--- a/static/testsheet/rev02_testcases_20200729.xlsx
+++ b/static/testsheet/rev02_testcases_20200729.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="272">
   <si>
     <t>No.</t>
   </si>
@@ -983,9 +983,6 @@
   <si>
     <t>1. Shows "Don't forget to input the password of the delete."
 2. Not allow only spaces.</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -2420,6 +2417,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2429,135 +2471,93 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2629,9 +2629,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3044,7 +3041,7 @@
       <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3064,13 +3061,11 @@
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
-      <c r="E1" s="11" t="s">
-        <v>272</v>
-      </c>
+      <c r="E1" s="11"/>
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="2:14" ht="18">
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="83" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="86" t="s">
@@ -3082,52 +3077,52 @@
       <c r="E2" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="89" t="s">
+      <c r="F2" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="79" t="s">
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="94" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15.6" customHeight="1">
-      <c r="B3" s="96"/>
+      <c r="B3" s="84"/>
       <c r="C3" s="87"/>
       <c r="D3" s="87"/>
       <c r="E3" s="87"/>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="82" t="s">
+      <c r="G3" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="85"/>
-      <c r="J3" s="84" t="s">
+      <c r="I3" s="98"/>
+      <c r="J3" s="97" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="85"/>
-      <c r="L3" s="84" t="s">
+      <c r="K3" s="98"/>
+      <c r="L3" s="97" t="s">
         <v>81</v>
       </c>
-      <c r="M3" s="85"/>
-      <c r="N3" s="80"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="95"/>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B4" s="97"/>
+      <c r="B4" s="85"/>
       <c r="C4" s="88"/>
       <c r="D4" s="88"/>
       <c r="E4" s="88"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
       <c r="H4" s="26" t="s">
         <v>14</v>
       </c>
@@ -3146,7 +3141,7 @@
       <c r="M4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="81"/>
+      <c r="N4" s="96"/>
     </row>
     <row r="5" spans="2:14" ht="72.599999999999994" thickTop="1">
       <c r="B5" s="5">
@@ -3175,7 +3170,7 @@
       <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="80" t="s">
         <v>55</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -3198,7 +3193,7 @@
       <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="93"/>
+      <c r="C7" s="81"/>
       <c r="D7" s="3" t="s">
         <v>72</v>
       </c>
@@ -3219,7 +3214,7 @@
       <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="C8" s="93"/>
+      <c r="C8" s="81"/>
       <c r="D8" s="3" t="s">
         <v>99</v>
       </c>
@@ -3240,7 +3235,7 @@
       <c r="B9" s="5">
         <v>5</v>
       </c>
-      <c r="C9" s="94"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="3" t="s">
         <v>73</v>
       </c>
@@ -3261,7 +3256,7 @@
       <c r="B10" s="5">
         <v>6</v>
       </c>
-      <c r="C10" s="93" t="s">
+      <c r="C10" s="81" t="s">
         <v>103</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -3284,7 +3279,7 @@
       <c r="B11" s="5">
         <v>7</v>
       </c>
-      <c r="C11" s="93"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="3" t="s">
         <v>110</v>
       </c>
@@ -3305,7 +3300,7 @@
       <c r="B12" s="5">
         <v>8</v>
       </c>
-      <c r="C12" s="93"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="3" t="s">
         <v>105</v>
       </c>
@@ -3326,7 +3321,7 @@
       <c r="B13" s="5">
         <v>9</v>
       </c>
-      <c r="C13" s="92" t="s">
+      <c r="C13" s="80" t="s">
         <v>107</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -3349,7 +3344,7 @@
       <c r="B14" s="5">
         <v>10</v>
       </c>
-      <c r="C14" s="93"/>
+      <c r="C14" s="81"/>
       <c r="D14" s="3" t="s">
         <v>178</v>
       </c>
@@ -3370,7 +3365,7 @@
       <c r="B15" s="5">
         <v>11</v>
       </c>
-      <c r="C15" s="92" t="s">
+      <c r="C15" s="80" t="s">
         <v>157</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -3393,7 +3388,7 @@
       <c r="B16" s="5">
         <v>12</v>
       </c>
-      <c r="C16" s="93"/>
+      <c r="C16" s="81"/>
       <c r="D16" s="3" t="s">
         <v>159</v>
       </c>
@@ -3414,7 +3409,7 @@
       <c r="B17" s="5">
         <v>13</v>
       </c>
-      <c r="C17" s="93"/>
+      <c r="C17" s="81"/>
       <c r="D17" s="3" t="s">
         <v>120</v>
       </c>
@@ -3435,7 +3430,7 @@
       <c r="B18" s="5">
         <v>14</v>
       </c>
-      <c r="C18" s="93"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="3" t="s">
         <v>160</v>
       </c>
@@ -3456,7 +3451,7 @@
       <c r="B19" s="5">
         <v>15</v>
       </c>
-      <c r="C19" s="93"/>
+      <c r="C19" s="81"/>
       <c r="D19" s="3" t="s">
         <v>123</v>
       </c>
@@ -3477,7 +3472,7 @@
       <c r="B20" s="5">
         <v>16</v>
       </c>
-      <c r="C20" s="93"/>
+      <c r="C20" s="81"/>
       <c r="D20" s="3" t="s">
         <v>163</v>
       </c>
@@ -3498,7 +3493,7 @@
       <c r="B21" s="5">
         <v>17</v>
       </c>
-      <c r="C21" s="93"/>
+      <c r="C21" s="81"/>
       <c r="D21" s="3" t="s">
         <v>125</v>
       </c>
@@ -3519,7 +3514,7 @@
       <c r="B22" s="5">
         <v>18</v>
       </c>
-      <c r="C22" s="93"/>
+      <c r="C22" s="81"/>
       <c r="D22" s="3" t="s">
         <v>155</v>
       </c>
@@ -3540,7 +3535,7 @@
       <c r="B23" s="5">
         <v>19</v>
       </c>
-      <c r="C23" s="93"/>
+      <c r="C23" s="81"/>
       <c r="D23" s="3" t="s">
         <v>126</v>
       </c>
@@ -3561,7 +3556,7 @@
       <c r="B24" s="5">
         <v>20</v>
       </c>
-      <c r="C24" s="93"/>
+      <c r="C24" s="81"/>
       <c r="D24" s="3" t="s">
         <v>130</v>
       </c>
@@ -3582,7 +3577,7 @@
       <c r="B25" s="5">
         <v>21</v>
       </c>
-      <c r="C25" s="93"/>
+      <c r="C25" s="81"/>
       <c r="D25" s="3" t="s">
         <v>169</v>
       </c>
@@ -3603,7 +3598,7 @@
       <c r="B26" s="5">
         <v>22</v>
       </c>
-      <c r="C26" s="93"/>
+      <c r="C26" s="81"/>
       <c r="D26" s="3" t="s">
         <v>133</v>
       </c>
@@ -3624,7 +3619,7 @@
       <c r="B27" s="5">
         <v>23</v>
       </c>
-      <c r="C27" s="93"/>
+      <c r="C27" s="81"/>
       <c r="D27" s="3" t="s">
         <v>142</v>
       </c>
@@ -3645,7 +3640,7 @@
       <c r="B28" s="5">
         <v>24</v>
       </c>
-      <c r="C28" s="93"/>
+      <c r="C28" s="81"/>
       <c r="D28" s="3" t="s">
         <v>167</v>
       </c>
@@ -3666,7 +3661,7 @@
       <c r="B29" s="5">
         <v>25</v>
       </c>
-      <c r="C29" s="93"/>
+      <c r="C29" s="81"/>
       <c r="D29" s="3" t="s">
         <v>170</v>
       </c>
@@ -3687,7 +3682,7 @@
       <c r="B30" s="5">
         <v>26</v>
       </c>
-      <c r="C30" s="93"/>
+      <c r="C30" s="81"/>
       <c r="D30" s="3" t="s">
         <v>145</v>
       </c>
@@ -3708,7 +3703,7 @@
       <c r="B31" s="5">
         <v>27</v>
       </c>
-      <c r="C31" s="93"/>
+      <c r="C31" s="81"/>
       <c r="D31" s="3" t="s">
         <v>142</v>
       </c>
@@ -3729,7 +3724,7 @@
       <c r="B32" s="5">
         <v>28</v>
       </c>
-      <c r="C32" s="93"/>
+      <c r="C32" s="81"/>
       <c r="D32" s="3" t="s">
         <v>167</v>
       </c>
@@ -3750,7 +3745,7 @@
       <c r="B33" s="5">
         <v>29</v>
       </c>
-      <c r="C33" s="93"/>
+      <c r="C33" s="81"/>
       <c r="D33" s="3" t="s">
         <v>175</v>
       </c>
@@ -3771,7 +3766,7 @@
       <c r="B34" s="5">
         <v>30</v>
       </c>
-      <c r="C34" s="93"/>
+      <c r="C34" s="81"/>
       <c r="D34" s="3" t="s">
         <v>151</v>
       </c>
@@ -3792,7 +3787,7 @@
       <c r="B35" s="5">
         <v>31</v>
       </c>
-      <c r="C35" s="93"/>
+      <c r="C35" s="81"/>
       <c r="D35" s="3" t="s">
         <v>174</v>
       </c>
@@ -3813,7 +3808,7 @@
       <c r="B36" s="5">
         <v>32</v>
       </c>
-      <c r="C36" s="94"/>
+      <c r="C36" s="82"/>
       <c r="D36" s="3" t="s">
         <v>154</v>
       </c>
@@ -3834,7 +3829,7 @@
       <c r="B37" s="5">
         <v>33</v>
       </c>
-      <c r="C37" s="92" t="s">
+      <c r="C37" s="80" t="s">
         <v>176</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -3857,7 +3852,7 @@
       <c r="B38" s="5">
         <v>34</v>
       </c>
-      <c r="C38" s="93"/>
+      <c r="C38" s="81"/>
       <c r="D38" s="3" t="s">
         <v>113</v>
       </c>
@@ -3878,7 +3873,7 @@
       <c r="B39" s="5">
         <v>35</v>
       </c>
-      <c r="C39" s="94"/>
+      <c r="C39" s="82"/>
       <c r="D39" s="3" t="s">
         <v>114</v>
       </c>
@@ -3899,7 +3894,7 @@
       <c r="B40" s="5">
         <v>36</v>
       </c>
-      <c r="C40" s="92" t="s">
+      <c r="C40" s="80" t="s">
         <v>117</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -3922,7 +3917,7 @@
       <c r="B41" s="5">
         <v>37</v>
       </c>
-      <c r="C41" s="93"/>
+      <c r="C41" s="81"/>
       <c r="D41" s="3" t="s">
         <v>121</v>
       </c>
@@ -3943,7 +3938,7 @@
       <c r="B42" s="5">
         <v>38</v>
       </c>
-      <c r="C42" s="93"/>
+      <c r="C42" s="81"/>
       <c r="D42" s="3" t="s">
         <v>120</v>
       </c>
@@ -3964,7 +3959,7 @@
       <c r="B43" s="5">
         <v>39</v>
       </c>
-      <c r="C43" s="93"/>
+      <c r="C43" s="81"/>
       <c r="D43" s="3" t="s">
         <v>122</v>
       </c>
@@ -3985,7 +3980,7 @@
       <c r="B44" s="5">
         <v>40</v>
       </c>
-      <c r="C44" s="93"/>
+      <c r="C44" s="81"/>
       <c r="D44" s="3" t="s">
         <v>123</v>
       </c>
@@ -4006,7 +4001,7 @@
       <c r="B45" s="5">
         <v>41</v>
       </c>
-      <c r="C45" s="93"/>
+      <c r="C45" s="81"/>
       <c r="D45" s="3" t="s">
         <v>124</v>
       </c>
@@ -4027,7 +4022,7 @@
       <c r="B46" s="5">
         <v>42</v>
       </c>
-      <c r="C46" s="93"/>
+      <c r="C46" s="81"/>
       <c r="D46" s="3" t="s">
         <v>125</v>
       </c>
@@ -4048,7 +4043,7 @@
       <c r="B47" s="5">
         <v>43</v>
       </c>
-      <c r="C47" s="93"/>
+      <c r="C47" s="81"/>
       <c r="D47" s="3" t="s">
         <v>155</v>
       </c>
@@ -4069,7 +4064,7 @@
       <c r="B48" s="5">
         <v>44</v>
       </c>
-      <c r="C48" s="93"/>
+      <c r="C48" s="81"/>
       <c r="D48" s="3" t="s">
         <v>166</v>
       </c>
@@ -4090,7 +4085,7 @@
       <c r="B49" s="5">
         <v>45</v>
       </c>
-      <c r="C49" s="93"/>
+      <c r="C49" s="81"/>
       <c r="D49" s="3" t="s">
         <v>130</v>
       </c>
@@ -4111,7 +4106,7 @@
       <c r="B50" s="5">
         <v>46</v>
       </c>
-      <c r="C50" s="93"/>
+      <c r="C50" s="81"/>
       <c r="D50" s="3" t="s">
         <v>134</v>
       </c>
@@ -4132,7 +4127,7 @@
       <c r="B51" s="5">
         <v>47</v>
       </c>
-      <c r="C51" s="93"/>
+      <c r="C51" s="81"/>
       <c r="D51" s="3" t="s">
         <v>133</v>
       </c>
@@ -4153,7 +4148,7 @@
       <c r="B52" s="5">
         <v>48</v>
       </c>
-      <c r="C52" s="93"/>
+      <c r="C52" s="81"/>
       <c r="D52" s="3" t="s">
         <v>135</v>
       </c>
@@ -4174,7 +4169,7 @@
       <c r="B53" s="5">
         <v>49</v>
       </c>
-      <c r="C53" s="93"/>
+      <c r="C53" s="81"/>
       <c r="D53" s="3" t="s">
         <v>142</v>
       </c>
@@ -4195,7 +4190,7 @@
       <c r="B54" s="5">
         <v>50</v>
       </c>
-      <c r="C54" s="93"/>
+      <c r="C54" s="81"/>
       <c r="D54" s="3" t="s">
         <v>167</v>
       </c>
@@ -4216,7 +4211,7 @@
       <c r="B55" s="5">
         <v>51</v>
       </c>
-      <c r="C55" s="93"/>
+      <c r="C55" s="81"/>
       <c r="D55" s="3" t="s">
         <v>144</v>
       </c>
@@ -4237,7 +4232,7 @@
       <c r="B56" s="5">
         <v>52</v>
       </c>
-      <c r="C56" s="93"/>
+      <c r="C56" s="81"/>
       <c r="D56" s="3" t="s">
         <v>145</v>
       </c>
@@ -4258,7 +4253,7 @@
       <c r="B57" s="5">
         <v>53</v>
       </c>
-      <c r="C57" s="93"/>
+      <c r="C57" s="81"/>
       <c r="D57" s="3" t="s">
         <v>147</v>
       </c>
@@ -4279,7 +4274,7 @@
       <c r="B58" s="5">
         <v>54</v>
       </c>
-      <c r="C58" s="93"/>
+      <c r="C58" s="81"/>
       <c r="D58" s="3" t="s">
         <v>142</v>
       </c>
@@ -4300,7 +4295,7 @@
       <c r="B59" s="5">
         <v>55</v>
       </c>
-      <c r="C59" s="93"/>
+      <c r="C59" s="81"/>
       <c r="D59" s="3" t="s">
         <v>167</v>
       </c>
@@ -4321,7 +4316,7 @@
       <c r="B60" s="5">
         <v>56</v>
       </c>
-      <c r="C60" s="93"/>
+      <c r="C60" s="81"/>
       <c r="D60" s="3" t="s">
         <v>149</v>
       </c>
@@ -4342,7 +4337,7 @@
       <c r="B61" s="5">
         <v>57</v>
       </c>
-      <c r="C61" s="93"/>
+      <c r="C61" s="81"/>
       <c r="D61" s="3" t="s">
         <v>151</v>
       </c>
@@ -4363,7 +4358,7 @@
       <c r="B62" s="5">
         <v>58</v>
       </c>
-      <c r="C62" s="93"/>
+      <c r="C62" s="81"/>
       <c r="D62" s="3" t="s">
         <v>153</v>
       </c>
@@ -4384,7 +4379,7 @@
       <c r="B63" s="5">
         <v>59</v>
       </c>
-      <c r="C63" s="94"/>
+      <c r="C63" s="82"/>
       <c r="D63" s="3" t="s">
         <v>154</v>
       </c>
@@ -4405,7 +4400,7 @@
       <c r="B64" s="5">
         <v>60</v>
       </c>
-      <c r="C64" s="92" t="s">
+      <c r="C64" s="80" t="s">
         <v>193</v>
       </c>
       <c r="D64" s="3" t="s">
@@ -4428,7 +4423,7 @@
       <c r="B65" s="5">
         <v>61</v>
       </c>
-      <c r="C65" s="93"/>
+      <c r="C65" s="81"/>
       <c r="D65" s="3" t="s">
         <v>196</v>
       </c>
@@ -4449,7 +4444,7 @@
       <c r="B66" s="5">
         <v>62</v>
       </c>
-      <c r="C66" s="94"/>
+      <c r="C66" s="82"/>
       <c r="D66" s="3" t="s">
         <v>206</v>
       </c>
@@ -4470,7 +4465,7 @@
       <c r="B67" s="5">
         <v>63</v>
       </c>
-      <c r="C67" s="92" t="s">
+      <c r="C67" s="80" t="s">
         <v>108</v>
       </c>
       <c r="D67" s="3" t="s">
@@ -4493,7 +4488,7 @@
       <c r="B68" s="5">
         <v>64</v>
       </c>
-      <c r="C68" s="93"/>
+      <c r="C68" s="81"/>
       <c r="D68" s="3" t="s">
         <v>256</v>
       </c>
@@ -4514,7 +4509,7 @@
       <c r="B69" s="5">
         <v>65</v>
       </c>
-      <c r="C69" s="93"/>
+      <c r="C69" s="81"/>
       <c r="D69" s="3" t="s">
         <v>109</v>
       </c>
@@ -4535,7 +4530,7 @@
       <c r="B70" s="5">
         <v>66</v>
       </c>
-      <c r="C70" s="93"/>
+      <c r="C70" s="81"/>
       <c r="D70" s="3" t="s">
         <v>17</v>
       </c>
@@ -4556,7 +4551,7 @@
       <c r="B71" s="5">
         <v>67</v>
       </c>
-      <c r="C71" s="93"/>
+      <c r="C71" s="81"/>
       <c r="D71" s="3" t="s">
         <v>258</v>
       </c>
@@ -4577,7 +4572,7 @@
       <c r="B72" s="5">
         <v>68</v>
       </c>
-      <c r="C72" s="94"/>
+      <c r="C72" s="82"/>
       <c r="D72" s="3" t="s">
         <v>78</v>
       </c>
@@ -4619,6 +4614,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="C6:C9"/>
     <mergeCell ref="C67:C72"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -4628,16 +4633,6 @@
     <mergeCell ref="C15:C36"/>
     <mergeCell ref="C37:C39"/>
     <mergeCell ref="C64:C66"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F2:M2"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:M73">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
@@ -4660,8 +4655,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4679,12 +4674,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="23.4">
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="100" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
       <c r="F1" s="51"/>
       <c r="G1" s="40"/>
       <c r="H1" s="40"/>
@@ -4692,12 +4687,12 @@
       <c r="J1" s="40"/>
     </row>
     <row r="2" spans="2:12" ht="23.4" customHeight="1">
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="101" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
       <c r="F2" s="52"/>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
@@ -4705,10 +4700,10 @@
       <c r="J2" s="41"/>
     </row>
     <row r="3" spans="2:12" ht="23.4" customHeight="1">
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
       <c r="F3" s="52"/>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
@@ -4716,10 +4711,10 @@
       <c r="J3" s="41"/>
     </row>
     <row r="4" spans="2:12" ht="23.4" customHeight="1">
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
       <c r="F4" s="52"/>
       <c r="G4" s="41"/>
       <c r="H4" s="41"/>
@@ -4727,10 +4722,10 @@
       <c r="J4" s="41"/>
     </row>
     <row r="5" spans="2:12" ht="37.799999999999997" customHeight="1">
-      <c r="B5" s="124"/>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="124"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
       <c r="F5" s="53"/>
       <c r="G5" s="42"/>
       <c r="H5" s="42"/>
@@ -4738,14 +4733,14 @@
       <c r="J5" s="42"/>
     </row>
     <row r="7" spans="2:12" ht="21.6" thickBot="1">
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="116" t="s">
         <v>201</v>
       </c>
-      <c r="C7" s="117"/>
-      <c r="D7" s="117"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
     </row>
     <row r="8" spans="2:12" ht="18.600000000000001" thickBot="1">
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="83" t="s">
         <v>229</v>
       </c>
       <c r="C8" s="86" t="s">
@@ -4754,29 +4749,29 @@
       <c r="D8" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="119" t="s">
+      <c r="E8" s="104" t="s">
         <v>221</v>
       </c>
-      <c r="F8" s="79" t="s">
+      <c r="F8" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="121" t="s">
+      <c r="G8" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="121"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="122"/>
-      <c r="L8" s="79" t="s">
+      <c r="H8" s="106"/>
+      <c r="I8" s="106"/>
+      <c r="J8" s="106"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="94" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="15" thickBot="1">
-      <c r="B9" s="118"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="113"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="99"/>
       <c r="G9" s="62" t="s">
         <v>5</v>
       </c>
@@ -4792,19 +4787,19 @@
       <c r="K9" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="L9" s="113"/>
+      <c r="L9" s="99"/>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="112" t="s">
+      <c r="B10" s="109" t="s">
         <v>207</v>
       </c>
-      <c r="C10" s="108" t="s">
+      <c r="C10" s="120" t="s">
         <v>227</v>
       </c>
       <c r="D10" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="E10" s="106" t="s">
+      <c r="E10" s="121" t="s">
         <v>212</v>
       </c>
       <c r="F10" s="50" t="s">
@@ -4828,12 +4823,12 @@
       <c r="L10" s="71"/>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="98"/>
-      <c r="C11" s="101"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="118"/>
       <c r="D11" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E11" s="93"/>
+      <c r="E11" s="81"/>
       <c r="F11" s="3" t="s">
         <v>224</v>
       </c>
@@ -4846,11 +4841,11 @@
     </row>
     <row r="12" spans="2:12" ht="28.8">
       <c r="B12" s="111"/>
-      <c r="C12" s="109"/>
+      <c r="C12" s="119"/>
       <c r="D12" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E12" s="94"/>
+      <c r="E12" s="82"/>
       <c r="F12" s="3" t="s">
         <v>268</v>
       </c>
@@ -4862,16 +4857,16 @@
       <c r="L12" s="77"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="112" t="s">
         <v>209</v>
       </c>
-      <c r="C13" s="100" t="s">
+      <c r="C13" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E13" s="103" t="s">
+      <c r="E13" s="108" t="s">
         <v>212</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -4885,12 +4880,12 @@
       <c r="L13" s="77"/>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="98"/>
-      <c r="C14" s="101"/>
+      <c r="B14" s="110"/>
+      <c r="C14" s="118"/>
       <c r="D14" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E14" s="103"/>
+      <c r="E14" s="108"/>
       <c r="F14" s="3" t="s">
         <v>224</v>
       </c>
@@ -4903,11 +4898,11 @@
     </row>
     <row r="15" spans="2:12" ht="43.2">
       <c r="B15" s="111"/>
-      <c r="C15" s="109"/>
+      <c r="C15" s="119"/>
       <c r="D15" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E15" s="103"/>
+      <c r="E15" s="108"/>
       <c r="F15" s="3" t="s">
         <v>267</v>
       </c>
@@ -4919,16 +4914,16 @@
       <c r="L15" s="77"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="110" t="s">
+      <c r="B16" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="C16" s="100" t="s">
+      <c r="C16" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E16" s="103" t="s">
+      <c r="E16" s="108" t="s">
         <v>213</v>
       </c>
       <c r="F16" s="3" t="s">
@@ -4942,12 +4937,12 @@
       <c r="L16" s="77"/>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="98"/>
-      <c r="C17" s="101"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="118"/>
       <c r="D17" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E17" s="103"/>
+      <c r="E17" s="108"/>
       <c r="F17" s="3" t="s">
         <v>224</v>
       </c>
@@ -4960,11 +4955,11 @@
     </row>
     <row r="18" spans="2:12">
       <c r="B18" s="111"/>
-      <c r="C18" s="109"/>
+      <c r="C18" s="119"/>
       <c r="D18" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E18" s="103"/>
+      <c r="E18" s="108"/>
       <c r="F18" s="3" t="s">
         <v>232</v>
       </c>
@@ -4976,16 +4971,16 @@
       <c r="L18" s="77"/>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="110" t="s">
+      <c r="B19" s="112" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="100" t="s">
+      <c r="C19" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E19" s="92" t="s">
+      <c r="E19" s="80" t="s">
         <v>216</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -4999,12 +4994,12 @@
       <c r="L19" s="77"/>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="98"/>
-      <c r="C20" s="101"/>
+      <c r="B20" s="110"/>
+      <c r="C20" s="118"/>
       <c r="D20" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="E20" s="93"/>
+      <c r="E20" s="81"/>
       <c r="F20" s="3" t="s">
         <v>234</v>
       </c>
@@ -5017,11 +5012,11 @@
     </row>
     <row r="21" spans="2:12">
       <c r="B21" s="111"/>
-      <c r="C21" s="109"/>
+      <c r="C21" s="119"/>
       <c r="D21" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="E21" s="94"/>
+      <c r="E21" s="82"/>
       <c r="F21" s="3" t="s">
         <v>242</v>
       </c>
@@ -5033,16 +5028,16 @@
       <c r="L21" s="77"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="110" t="s">
+      <c r="B22" s="112" t="s">
         <v>217</v>
       </c>
-      <c r="C22" s="100" t="s">
+      <c r="C22" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E22" s="103" t="s">
+      <c r="E22" s="108" t="s">
         <v>212</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -5056,12 +5051,12 @@
       <c r="L22" s="77"/>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="98"/>
-      <c r="C23" s="101"/>
+      <c r="B23" s="110"/>
+      <c r="C23" s="118"/>
       <c r="D23" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E23" s="103"/>
+      <c r="E23" s="108"/>
       <c r="F23" s="3" t="s">
         <v>224</v>
       </c>
@@ -5074,11 +5069,11 @@
     </row>
     <row r="24" spans="2:12" ht="57.6">
       <c r="B24" s="111"/>
-      <c r="C24" s="109"/>
+      <c r="C24" s="119"/>
       <c r="D24" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E24" s="103"/>
+      <c r="E24" s="108"/>
       <c r="F24" s="3" t="s">
         <v>269</v>
       </c>
@@ -5090,16 +5085,16 @@
       <c r="L24" s="77"/>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="98" t="s">
+      <c r="B25" s="110" t="s">
         <v>218</v>
       </c>
-      <c r="C25" s="100" t="s">
+      <c r="C25" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E25" s="103" t="s">
+      <c r="E25" s="108" t="s">
         <v>212</v>
       </c>
       <c r="F25" s="3" t="s">
@@ -5113,12 +5108,12 @@
       <c r="L25" s="77"/>
     </row>
     <row r="26" spans="2:12">
-      <c r="B26" s="98"/>
-      <c r="C26" s="101"/>
+      <c r="B26" s="110"/>
+      <c r="C26" s="118"/>
       <c r="D26" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E26" s="103"/>
+      <c r="E26" s="108"/>
       <c r="F26" s="3" t="s">
         <v>224</v>
       </c>
@@ -5130,12 +5125,12 @@
       <c r="L26" s="77"/>
     </row>
     <row r="27" spans="2:12" ht="57.6">
-      <c r="B27" s="98"/>
-      <c r="C27" s="109"/>
+      <c r="B27" s="110"/>
+      <c r="C27" s="119"/>
       <c r="D27" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E27" s="103"/>
+      <c r="E27" s="108"/>
       <c r="F27" s="3" t="s">
         <v>269</v>
       </c>
@@ -5147,16 +5142,16 @@
       <c r="L27" s="77"/>
     </row>
     <row r="28" spans="2:12">
-      <c r="B28" s="110" t="s">
+      <c r="B28" s="112" t="s">
         <v>219</v>
       </c>
-      <c r="C28" s="100" t="s">
+      <c r="C28" s="117" t="s">
         <v>228</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E28" s="103" t="s">
+      <c r="E28" s="108" t="s">
         <v>212</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -5170,12 +5165,12 @@
       <c r="L28" s="77"/>
     </row>
     <row r="29" spans="2:12">
-      <c r="B29" s="98"/>
-      <c r="C29" s="101"/>
+      <c r="B29" s="110"/>
+      <c r="C29" s="118"/>
       <c r="D29" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E29" s="103"/>
+      <c r="E29" s="108"/>
       <c r="F29" s="3" t="s">
         <v>224</v>
       </c>
@@ -5188,11 +5183,11 @@
     </row>
     <row r="30" spans="2:12" ht="43.2">
       <c r="B30" s="111"/>
-      <c r="C30" s="109"/>
+      <c r="C30" s="119"/>
       <c r="D30" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E30" s="103"/>
+      <c r="E30" s="108"/>
       <c r="F30" s="3" t="s">
         <v>270</v>
       </c>
@@ -5204,16 +5199,16 @@
       <c r="L30" s="77"/>
     </row>
     <row r="31" spans="2:12" ht="28.8">
-      <c r="B31" s="98" t="s">
+      <c r="B31" s="110" t="s">
         <v>220</v>
       </c>
-      <c r="C31" s="100" t="s">
+      <c r="C31" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E31" s="103" t="s">
+      <c r="E31" s="108" t="s">
         <v>220</v>
       </c>
       <c r="F31" s="3" t="s">
@@ -5227,12 +5222,12 @@
       <c r="L31" s="77"/>
     </row>
     <row r="32" spans="2:12" ht="28.8">
-      <c r="B32" s="98"/>
-      <c r="C32" s="101"/>
+      <c r="B32" s="110"/>
+      <c r="C32" s="118"/>
       <c r="D32" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E32" s="92"/>
+      <c r="E32" s="80"/>
       <c r="F32" s="78" t="s">
         <v>245</v>
       </c>
@@ -5244,12 +5239,12 @@
       <c r="L32" s="77"/>
     </row>
     <row r="33" spans="2:12" ht="29.4" thickBot="1">
-      <c r="B33" s="99"/>
-      <c r="C33" s="102"/>
+      <c r="B33" s="123"/>
+      <c r="C33" s="124"/>
       <c r="D33" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="E33" s="104"/>
+      <c r="E33" s="122"/>
       <c r="F33" s="4" t="s">
         <v>271</v>
       </c>
@@ -5271,14 +5266,14 @@
       <c r="L33" s="46"/>
     </row>
     <row r="35" spans="2:12" ht="21.6" thickBot="1">
-      <c r="B35" s="117" t="s">
+      <c r="B35" s="116" t="s">
         <v>202</v>
       </c>
-      <c r="C35" s="117"/>
-      <c r="D35" s="117"/>
+      <c r="C35" s="116"/>
+      <c r="D35" s="116"/>
     </row>
     <row r="36" spans="2:12" ht="18.600000000000001" thickBot="1">
-      <c r="B36" s="95" t="s">
+      <c r="B36" s="83" t="s">
         <v>229</v>
       </c>
       <c r="C36" s="86" t="s">
@@ -5287,29 +5282,29 @@
       <c r="D36" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="E36" s="119" t="s">
+      <c r="E36" s="104" t="s">
         <v>221</v>
       </c>
-      <c r="F36" s="79" t="s">
+      <c r="F36" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="G36" s="121" t="s">
+      <c r="G36" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="H36" s="121"/>
-      <c r="I36" s="121"/>
-      <c r="J36" s="121"/>
-      <c r="K36" s="122"/>
-      <c r="L36" s="79" t="s">
+      <c r="H36" s="106"/>
+      <c r="I36" s="106"/>
+      <c r="J36" s="106"/>
+      <c r="K36" s="107"/>
+      <c r="L36" s="94" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="2:12" ht="18.600000000000001" customHeight="1" thickBot="1">
-      <c r="B37" s="118"/>
-      <c r="C37" s="105"/>
-      <c r="D37" s="105"/>
-      <c r="E37" s="120"/>
-      <c r="F37" s="113"/>
+      <c r="B37" s="102"/>
+      <c r="C37" s="103"/>
+      <c r="D37" s="103"/>
+      <c r="E37" s="105"/>
+      <c r="F37" s="99"/>
       <c r="G37" s="62" t="s">
         <v>5</v>
       </c>
@@ -5325,19 +5320,19 @@
       <c r="K37" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="L37" s="113"/>
+      <c r="L37" s="99"/>
     </row>
     <row r="38" spans="2:12">
-      <c r="B38" s="112" t="s">
+      <c r="B38" s="109" t="s">
         <v>207</v>
       </c>
-      <c r="C38" s="108" t="s">
+      <c r="C38" s="120" t="s">
         <v>227</v>
       </c>
       <c r="D38" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="E38" s="106" t="s">
+      <c r="E38" s="121" t="s">
         <v>212</v>
       </c>
       <c r="F38" s="50" t="s">
@@ -5361,12 +5356,12 @@
       <c r="L38" s="71"/>
     </row>
     <row r="39" spans="2:12">
-      <c r="B39" s="98"/>
-      <c r="C39" s="101"/>
+      <c r="B39" s="110"/>
+      <c r="C39" s="118"/>
       <c r="D39" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E39" s="93"/>
+      <c r="E39" s="81"/>
       <c r="F39" s="3" t="s">
         <v>224</v>
       </c>
@@ -5379,11 +5374,11 @@
     </row>
     <row r="40" spans="2:12">
       <c r="B40" s="111"/>
-      <c r="C40" s="109"/>
+      <c r="C40" s="119"/>
       <c r="D40" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E40" s="94"/>
+      <c r="E40" s="82"/>
       <c r="F40" s="3" t="s">
         <v>230</v>
       </c>
@@ -5395,16 +5390,16 @@
       <c r="L40" s="77"/>
     </row>
     <row r="41" spans="2:12">
-      <c r="B41" s="110" t="s">
+      <c r="B41" s="112" t="s">
         <v>209</v>
       </c>
-      <c r="C41" s="100" t="s">
+      <c r="C41" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E41" s="103" t="s">
+      <c r="E41" s="108" t="s">
         <v>212</v>
       </c>
       <c r="F41" s="3" t="s">
@@ -5418,12 +5413,12 @@
       <c r="L41" s="77"/>
     </row>
     <row r="42" spans="2:12">
-      <c r="B42" s="98"/>
-      <c r="C42" s="101"/>
+      <c r="B42" s="110"/>
+      <c r="C42" s="118"/>
       <c r="D42" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E42" s="103"/>
+      <c r="E42" s="108"/>
       <c r="F42" s="3" t="s">
         <v>224</v>
       </c>
@@ -5436,11 +5431,11 @@
     </row>
     <row r="43" spans="2:12" ht="28.8">
       <c r="B43" s="111"/>
-      <c r="C43" s="109"/>
+      <c r="C43" s="119"/>
       <c r="D43" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E43" s="103"/>
+      <c r="E43" s="108"/>
       <c r="F43" s="3" t="s">
         <v>231</v>
       </c>
@@ -5452,16 +5447,16 @@
       <c r="L43" s="77"/>
     </row>
     <row r="44" spans="2:12">
-      <c r="B44" s="110" t="s">
+      <c r="B44" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="C44" s="100" t="s">
+      <c r="C44" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E44" s="103" t="s">
+      <c r="E44" s="108" t="s">
         <v>213</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -5475,12 +5470,12 @@
       <c r="L44" s="77"/>
     </row>
     <row r="45" spans="2:12">
-      <c r="B45" s="98"/>
-      <c r="C45" s="101"/>
+      <c r="B45" s="110"/>
+      <c r="C45" s="118"/>
       <c r="D45" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E45" s="103"/>
+      <c r="E45" s="108"/>
       <c r="F45" s="3" t="s">
         <v>224</v>
       </c>
@@ -5493,11 +5488,11 @@
     </row>
     <row r="46" spans="2:12">
       <c r="B46" s="111"/>
-      <c r="C46" s="109"/>
+      <c r="C46" s="119"/>
       <c r="D46" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E46" s="103"/>
+      <c r="E46" s="108"/>
       <c r="F46" s="3" t="s">
         <v>232</v>
       </c>
@@ -5509,16 +5504,16 @@
       <c r="L46" s="77"/>
     </row>
     <row r="47" spans="2:12">
-      <c r="B47" s="110" t="s">
+      <c r="B47" s="112" t="s">
         <v>214</v>
       </c>
-      <c r="C47" s="100" t="s">
+      <c r="C47" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="E47" s="92" t="s">
+      <c r="E47" s="80" t="s">
         <v>216</v>
       </c>
       <c r="F47" s="3" t="s">
@@ -5533,11 +5528,11 @@
     </row>
     <row r="48" spans="2:12">
       <c r="B48" s="111"/>
-      <c r="C48" s="109"/>
+      <c r="C48" s="119"/>
       <c r="D48" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="E48" s="94"/>
+      <c r="E48" s="82"/>
       <c r="F48" s="3" t="s">
         <v>242</v>
       </c>
@@ -5549,16 +5544,16 @@
       <c r="L48" s="77"/>
     </row>
     <row r="49" spans="2:12">
-      <c r="B49" s="110" t="s">
+      <c r="B49" s="112" t="s">
         <v>217</v>
       </c>
-      <c r="C49" s="100" t="s">
+      <c r="C49" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E49" s="103" t="s">
+      <c r="E49" s="108" t="s">
         <v>212</v>
       </c>
       <c r="F49" s="3" t="s">
@@ -5572,12 +5567,12 @@
       <c r="L49" s="77"/>
     </row>
     <row r="50" spans="2:12">
-      <c r="B50" s="98"/>
-      <c r="C50" s="101"/>
+      <c r="B50" s="110"/>
+      <c r="C50" s="118"/>
       <c r="D50" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E50" s="103"/>
+      <c r="E50" s="108"/>
       <c r="F50" s="3" t="s">
         <v>224</v>
       </c>
@@ -5590,11 +5585,11 @@
     </row>
     <row r="51" spans="2:12" ht="43.2">
       <c r="B51" s="111"/>
-      <c r="C51" s="109"/>
+      <c r="C51" s="119"/>
       <c r="D51" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E51" s="103"/>
+      <c r="E51" s="108"/>
       <c r="F51" s="3" t="s">
         <v>243</v>
       </c>
@@ -5606,16 +5601,16 @@
       <c r="L51" s="77"/>
     </row>
     <row r="52" spans="2:12">
-      <c r="B52" s="98" t="s">
+      <c r="B52" s="110" t="s">
         <v>218</v>
       </c>
-      <c r="C52" s="100" t="s">
+      <c r="C52" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E52" s="103" t="s">
+      <c r="E52" s="108" t="s">
         <v>212</v>
       </c>
       <c r="F52" s="3" t="s">
@@ -5629,12 +5624,12 @@
       <c r="L52" s="77"/>
     </row>
     <row r="53" spans="2:12">
-      <c r="B53" s="98"/>
-      <c r="C53" s="101"/>
+      <c r="B53" s="110"/>
+      <c r="C53" s="118"/>
       <c r="D53" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E53" s="103"/>
+      <c r="E53" s="108"/>
       <c r="F53" s="3" t="s">
         <v>224</v>
       </c>
@@ -5646,12 +5641,12 @@
       <c r="L53" s="77"/>
     </row>
     <row r="54" spans="2:12" ht="43.2">
-      <c r="B54" s="98"/>
-      <c r="C54" s="109"/>
+      <c r="B54" s="110"/>
+      <c r="C54" s="119"/>
       <c r="D54" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E54" s="103"/>
+      <c r="E54" s="108"/>
       <c r="F54" s="3" t="s">
         <v>243</v>
       </c>
@@ -5663,16 +5658,16 @@
       <c r="L54" s="77"/>
     </row>
     <row r="55" spans="2:12">
-      <c r="B55" s="110" t="s">
+      <c r="B55" s="112" t="s">
         <v>219</v>
       </c>
-      <c r="C55" s="100" t="s">
+      <c r="C55" s="117" t="s">
         <v>228</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E55" s="103" t="s">
+      <c r="E55" s="108" t="s">
         <v>212</v>
       </c>
       <c r="F55" s="3" t="s">
@@ -5686,12 +5681,12 @@
       <c r="L55" s="77"/>
     </row>
     <row r="56" spans="2:12">
-      <c r="B56" s="98"/>
-      <c r="C56" s="101"/>
+      <c r="B56" s="110"/>
+      <c r="C56" s="118"/>
       <c r="D56" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E56" s="103"/>
+      <c r="E56" s="108"/>
       <c r="F56" s="3" t="s">
         <v>224</v>
       </c>
@@ -5704,11 +5699,11 @@
     </row>
     <row r="57" spans="2:12" ht="28.8">
       <c r="B57" s="111"/>
-      <c r="C57" s="109"/>
+      <c r="C57" s="119"/>
       <c r="D57" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E57" s="103"/>
+      <c r="E57" s="108"/>
       <c r="F57" s="3" t="s">
         <v>244</v>
       </c>
@@ -5720,16 +5715,16 @@
       <c r="L57" s="77"/>
     </row>
     <row r="58" spans="2:12" ht="28.8">
-      <c r="B58" s="98" t="s">
+      <c r="B58" s="110" t="s">
         <v>220</v>
       </c>
-      <c r="C58" s="100" t="s">
+      <c r="C58" s="117" t="s">
         <v>227</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E58" s="103" t="s">
+      <c r="E58" s="108" t="s">
         <v>220</v>
       </c>
       <c r="F58" s="3" t="s">
@@ -5743,12 +5738,12 @@
       <c r="L58" s="77"/>
     </row>
     <row r="59" spans="2:12" ht="28.8">
-      <c r="B59" s="98"/>
-      <c r="C59" s="101"/>
+      <c r="B59" s="110"/>
+      <c r="C59" s="118"/>
       <c r="D59" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E59" s="92"/>
+      <c r="E59" s="80"/>
       <c r="F59" s="78" t="s">
         <v>245</v>
       </c>
@@ -5760,12 +5755,12 @@
       <c r="L59" s="77"/>
     </row>
     <row r="60" spans="2:12" ht="14.4" customHeight="1" thickBot="1">
-      <c r="B60" s="99"/>
-      <c r="C60" s="102"/>
+      <c r="B60" s="123"/>
+      <c r="C60" s="124"/>
       <c r="D60" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="E60" s="104"/>
+      <c r="E60" s="122"/>
       <c r="F60" s="4" t="s">
         <v>246</v>
       </c>
@@ -5787,14 +5782,14 @@
       <c r="L60" s="46"/>
     </row>
     <row r="62" spans="2:12" ht="21.6" thickBot="1">
-      <c r="B62" s="117" t="s">
+      <c r="B62" s="116" t="s">
         <v>203</v>
       </c>
-      <c r="C62" s="117"/>
-      <c r="D62" s="117"/>
+      <c r="C62" s="116"/>
+      <c r="D62" s="116"/>
     </row>
     <row r="63" spans="2:12" ht="18.600000000000001" thickBot="1">
-      <c r="B63" s="95" t="s">
+      <c r="B63" s="83" t="s">
         <v>249</v>
       </c>
       <c r="C63" s="86" t="s">
@@ -5803,29 +5798,29 @@
       <c r="D63" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="E63" s="119" t="s">
+      <c r="E63" s="104" t="s">
         <v>221</v>
       </c>
-      <c r="F63" s="79" t="s">
+      <c r="F63" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="G63" s="121" t="s">
+      <c r="G63" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="H63" s="121"/>
-      <c r="I63" s="121"/>
-      <c r="J63" s="121"/>
-      <c r="K63" s="122"/>
-      <c r="L63" s="79" t="s">
+      <c r="H63" s="106"/>
+      <c r="I63" s="106"/>
+      <c r="J63" s="106"/>
+      <c r="K63" s="107"/>
+      <c r="L63" s="94" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="64" spans="2:12" ht="18.600000000000001" customHeight="1" thickBot="1">
-      <c r="B64" s="118"/>
-      <c r="C64" s="105"/>
-      <c r="D64" s="105"/>
-      <c r="E64" s="120"/>
-      <c r="F64" s="113"/>
+      <c r="B64" s="102"/>
+      <c r="C64" s="103"/>
+      <c r="D64" s="103"/>
+      <c r="E64" s="105"/>
+      <c r="F64" s="99"/>
       <c r="G64" s="62" t="s">
         <v>5</v>
       </c>
@@ -5841,19 +5836,19 @@
       <c r="K64" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="L64" s="113"/>
+      <c r="L64" s="99"/>
     </row>
     <row r="65" spans="2:12">
-      <c r="B65" s="114" t="s">
+      <c r="B65" s="113" t="s">
         <v>220</v>
       </c>
-      <c r="C65" s="108" t="s">
+      <c r="C65" s="120" t="s">
         <v>228</v>
       </c>
       <c r="D65" s="50" t="s">
         <v>250</v>
       </c>
-      <c r="E65" s="106" t="s">
+      <c r="E65" s="121" t="s">
         <v>220</v>
       </c>
       <c r="F65" s="50" t="s">
@@ -5867,12 +5862,12 @@
       <c r="L65" s="72"/>
     </row>
     <row r="66" spans="2:12" ht="28.8">
-      <c r="B66" s="115"/>
-      <c r="C66" s="101"/>
+      <c r="B66" s="114"/>
+      <c r="C66" s="118"/>
       <c r="D66" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="E66" s="93"/>
+      <c r="E66" s="81"/>
       <c r="F66" s="3" t="s">
         <v>253</v>
       </c>
@@ -5884,12 +5879,12 @@
       <c r="L66" s="45"/>
     </row>
     <row r="67" spans="2:12" ht="29.4" thickBot="1">
-      <c r="B67" s="116"/>
-      <c r="C67" s="102"/>
+      <c r="B67" s="115"/>
+      <c r="C67" s="124"/>
       <c r="D67" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="E67" s="107"/>
+      <c r="E67" s="125"/>
       <c r="F67" s="4" t="s">
         <v>253</v>
       </c>
@@ -5902,21 +5897,51 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E5"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="E58:E60"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="E55:E57"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C10:C12"/>
     <mergeCell ref="L63:L64"/>
     <mergeCell ref="B65:B67"/>
     <mergeCell ref="B7:D7"/>
@@ -5933,52 +5958,22 @@
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="B16:B18"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E5"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="E55:E57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="E58:E60"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="C65:C67"/>
   </mergeCells>
   <conditionalFormatting sqref="G10:K33 G38:K60 G65:K67">
     <cfRule type="cellIs" dxfId="2" priority="22" operator="equal">
@@ -6023,79 +6018,79 @@
       <c r="G1" s="40"/>
     </row>
     <row r="2" spans="2:8" ht="23.4" customHeight="1">
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
     </row>
     <row r="3" spans="2:8" ht="23.4" customHeight="1">
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
+      <c r="B3" s="135"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
     </row>
     <row r="4" spans="2:8" ht="23.4" customHeight="1">
-      <c r="B4" s="134"/>
-      <c r="C4" s="134"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
+      <c r="B4" s="135"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="135"/>
       <c r="F4" s="41"/>
       <c r="G4" s="41"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" thickBot="1">
-      <c r="B5" s="135"/>
-      <c r="C5" s="135"/>
-      <c r="D5" s="135"/>
-      <c r="E5" s="135"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
     </row>
     <row r="6" spans="2:8" ht="18" customHeight="1">
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="131" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="136" t="s">
+      <c r="C6" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="125" t="s">
+      <c r="D6" s="126" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="125" t="s">
+      <c r="E6" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="125" t="s">
+      <c r="F6" s="126" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="125" t="s">
+      <c r="G6" s="126" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="127" t="s">
+      <c r="H6" s="128" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.6" customHeight="1">
-      <c r="B7" s="131"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="128"/>
+      <c r="B7" s="132"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
+      <c r="H7" s="129"/>
     </row>
     <row r="8" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="B8" s="132"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="129"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="130"/>
     </row>
     <row r="9" spans="2:8" ht="30" customHeight="1" thickTop="1">
       <c r="B9" s="56" t="s">
@@ -6160,7 +6155,7 @@
   <dimension ref="B1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G13" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6183,79 +6178,79 @@
       <c r="G1" s="40"/>
     </row>
     <row r="2" spans="2:8" ht="23.4" customHeight="1">
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
     </row>
     <row r="3" spans="2:8" ht="23.4" customHeight="1">
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
+      <c r="B3" s="135"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
     </row>
     <row r="4" spans="2:8" ht="23.4" customHeight="1">
-      <c r="B4" s="134"/>
-      <c r="C4" s="134"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
+      <c r="B4" s="135"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="135"/>
       <c r="F4" s="41"/>
       <c r="G4" s="41"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" thickBot="1">
-      <c r="B5" s="135"/>
-      <c r="C5" s="135"/>
-      <c r="D5" s="135"/>
-      <c r="E5" s="135"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
     </row>
     <row r="6" spans="2:8" ht="18" customHeight="1">
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="131" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="136" t="s">
+      <c r="C6" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="125" t="s">
+      <c r="D6" s="126" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="125" t="s">
+      <c r="E6" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="F6" s="125" t="s">
+      <c r="F6" s="126" t="s">
         <v>181</v>
       </c>
-      <c r="G6" s="125" t="s">
+      <c r="G6" s="126" t="s">
         <v>182</v>
       </c>
-      <c r="H6" s="127" t="s">
+      <c r="H6" s="128" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.6" customHeight="1">
-      <c r="B7" s="131"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="128"/>
+      <c r="B7" s="132"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
+      <c r="H7" s="129"/>
     </row>
     <row r="8" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="B8" s="132"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="129"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="130"/>
     </row>
     <row r="9" spans="2:8" ht="30" customHeight="1" thickTop="1">
       <c r="B9" s="68" t="s">
@@ -6382,8 +6377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6457,7 +6452,7 @@
       <c r="B2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="79" t="s">
         <v>266</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -6564,7 +6559,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6598,100 +6593,100 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickTop="1">
       <c r="A1"/>
-      <c r="B1" s="137" t="s">
+      <c r="B1" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="140"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2"/>
-      <c r="B2" s="140" t="s">
+      <c r="B2" s="141" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="142"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="143"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3"/>
-      <c r="B3" s="140" t="s">
+      <c r="B3" s="141" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="142"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="143"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4"/>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="141" t="s">
         <v>205</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="142"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="143"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5"/>
-      <c r="B5" s="140"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="141"/>
-      <c r="E5" s="142"/>
+      <c r="B5" s="141"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="142"/>
+      <c r="E5" s="143"/>
     </row>
     <row r="6" spans="1:7" ht="15.6">
       <c r="A6"/>
-      <c r="B6" s="146" t="s">
+      <c r="B6" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="147"/>
-      <c r="D6" s="147"/>
-      <c r="E6" s="148"/>
+      <c r="C6" s="148"/>
+      <c r="D6" s="148"/>
+      <c r="E6" s="149"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7"/>
-      <c r="B7" s="140" t="s">
+      <c r="B7" s="141" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="141"/>
-      <c r="D7" s="141"/>
-      <c r="E7" s="142"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="142"/>
+      <c r="E7" s="143"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8"/>
-      <c r="B8" s="140" t="s">
+      <c r="B8" s="141" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="141"/>
-      <c r="D8" s="141"/>
-      <c r="E8" s="142"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="143"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9"/>
-      <c r="B9" s="140" t="s">
+      <c r="B9" s="141" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="141"/>
-      <c r="D9" s="141"/>
-      <c r="E9" s="142"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="143"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10"/>
-      <c r="B10" s="140" t="s">
+      <c r="B10" s="141" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="141"/>
-      <c r="D10" s="141"/>
-      <c r="E10" s="142"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="143"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1">
       <c r="A11"/>
-      <c r="B11" s="143" t="s">
+      <c r="B11" s="144" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="144"/>
-      <c r="D11" s="144"/>
-      <c r="E11" s="145"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="145"/>
+      <c r="E11" s="146"/>
     </row>
     <row r="12" spans="1:7" ht="15.6" thickTop="1" thickBot="1">
       <c r="A12"/>
@@ -6702,12 +6697,12 @@
     </row>
     <row r="13" spans="1:7" ht="24.6" thickTop="1" thickBot="1">
       <c r="A13"/>
-      <c r="B13" s="137" t="s">
+      <c r="B13" s="138" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="139"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="139"/>
+      <c r="E13" s="140"/>
     </row>
     <row r="14" spans="1:7" s="9" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="B14" s="22"/>
@@ -6851,12 +6846,12 @@
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="2:7" ht="24.6" thickTop="1" thickBot="1">
-      <c r="B22" s="137" t="s">
+      <c r="B22" s="138" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="139"/>
+      <c r="C22" s="139"/>
+      <c r="D22" s="139"/>
+      <c r="E22" s="140"/>
       <c r="F22" s="21"/>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" thickBot="1">

</xml_diff>